<commit_message>
SJT + SRI Plots
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/coding_sri_expert.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/sri coding/data/coding_sri_expert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\sri coding\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{4B117B54-8B1F-4930-8544-C8E3FF8A5375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{81312A99-61F6-4A30-A344-09D2B1A36643}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{4B117B54-8B1F-4930-8544-C8E3FF8A5375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{97AE1175-C184-4C6C-AA75-3B8035DFE225}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{62789846-DE95-45C1-A820-53E90CFB7279}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="21">
   <si>
     <t>chatting</t>
   </si>
@@ -78,13 +78,16 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Disturbing_Factor</t>
-  </si>
-  <si>
     <t>Dispersion_School</t>
   </si>
   <si>
     <t>Confident_Factor</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Disruption_Factor</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,13 +511,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1220,31 +1223,184 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B38" s="4"/>
+      <c r="A38" s="1">
+        <v>205</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1">
+        <v>9</v>
+      </c>
+      <c r="F38" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="4"/>
+      <c r="A39" s="1">
+        <v>205</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B40" s="4"/>
+      <c r="A40" s="1">
+        <v>205</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1">
+        <v>8</v>
+      </c>
+      <c r="F40" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="4"/>
+      <c r="A41" s="1">
+        <v>205</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="1">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1">
+        <v>9</v>
+      </c>
+      <c r="F41" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
+      <c r="A42" s="1">
+        <v>205</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="1">
+        <v>6</v>
+      </c>
+      <c r="E42" s="1">
+        <v>9</v>
+      </c>
+      <c r="F42" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="4"/>
+      <c r="A43" s="1">
+        <v>205</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
+        <v>9</v>
+      </c>
+      <c r="F43" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B44" s="4"/>
+      <c r="A44" s="1">
+        <v>205</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="4"/>
+      <c r="A45" s="1">
+        <v>205</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="1">
+        <v>7</v>
+      </c>
+      <c r="E45" s="1">
+        <v>6</v>
+      </c>
+      <c r="F45" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="46" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="3"/>
+      <c r="A46" s="2">
+        <v>205</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2">
+        <v>5</v>
+      </c>
+      <c r="E46" s="2">
+        <v>9</v>
+      </c>
+      <c r="F46" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>

</xml_diff>